<commit_message>
Created Object Repo folder for BWP
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/DisplayCFData.xlsx
+++ b/KatalonData/IWPTestData/DisplayCFData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5932" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7192" uniqueCount="922">
   <si>
     <t>Result</t>
   </si>
@@ -1861,6 +1861,951 @@
   </si>
   <si>
     <t>Tue Jul 29 21:03:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:30:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:31:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:32:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:33:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:34:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:35:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:35:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:36:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:37:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:38:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:40:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:40:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:42:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:43:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:44:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:45:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:45:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:47:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:48:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:49:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:49:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:50:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:51:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:52:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:53:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:54:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:55:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:59:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:00:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:01:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:02:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:03:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:04:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:05:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:06:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:08:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:09:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:09:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:11:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:12:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:13:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:14:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:15:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:16:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:17:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:18:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:19:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:20:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:22:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:23:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:24:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:26:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:27:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:27:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:28:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:29:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:30:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:31:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:32:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:33:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:34:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:36:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:37:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:38:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:39:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:40:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:40:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:41:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:42:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:43:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:44:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:47:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:48:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:48:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:49:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:50:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:51:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:52:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:53:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:55:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:56:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:57:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:58:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:59:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:00:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:00:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:02:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:03:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:04:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:05:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:07:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:08:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:09:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:10:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:11:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:12:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:13:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:14:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:15:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:17:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:18:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:19:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:21:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:21:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:22:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:24:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:25:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:26:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:27:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:27:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:29:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:30:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:32:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:33:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:34:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:35:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:36:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:36:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:37:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:41:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:42:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:44:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:45:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:46:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:47:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:48:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:49:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:50:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:51:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:53:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:53:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:55:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:56:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:57:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:59:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:00:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:01:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:03:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:03:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:04:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:06:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:07:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:08:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:09:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:10:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:11:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:12:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:13:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:14:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:15:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:16:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:08:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:10:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:11:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:12:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:14:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:16:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:17:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:19:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:21:09 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -2364,10 +3309,10 @@
     </row>
     <row ht="30" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
+        <v>607</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -2431,10 +3376,10 @@
     </row>
     <row ht="30" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>548</v>
+        <v>608</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -2498,10 +3443,10 @@
     </row>
     <row ht="30" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>549</v>
+        <v>609</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -2565,10 +3510,10 @@
     </row>
     <row ht="30" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>550</v>
+        <v>610</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -2632,10 +3577,10 @@
     </row>
     <row ht="30" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>551</v>
+        <v>611</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -2699,10 +3644,10 @@
     </row>
     <row ht="30" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>552</v>
+        <v>612</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -2766,10 +3711,10 @@
     </row>
     <row ht="30" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>553</v>
+        <v>613</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -2833,10 +3778,10 @@
     </row>
     <row ht="30" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -2900,10 +3845,10 @@
     </row>
     <row ht="30" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>555</v>
+        <v>615</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2970,7 +3915,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -3034,10 +3979,10 @@
     </row>
     <row ht="30" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>557</v>
+        <v>617</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -3104,7 +4049,7 @@
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>558</v>
+        <v>618</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -3168,10 +4113,10 @@
     </row>
     <row ht="30" r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>559</v>
+        <v>619</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -3235,10 +4180,10 @@
     </row>
     <row ht="30" r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>560</v>
+        <v>620</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -3302,10 +4247,10 @@
     </row>
     <row ht="30" r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>561</v>
+        <v>621</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -3369,10 +4314,10 @@
     </row>
     <row ht="30" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>562</v>
+        <v>622</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -3439,7 +4384,7 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>563</v>
+        <v>623</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -3503,10 +4448,10 @@
     </row>
     <row ht="30" r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>564</v>
+        <v>624</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -3570,10 +4515,10 @@
     </row>
     <row ht="30" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>565</v>
+        <v>625</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -3637,10 +4582,10 @@
     </row>
     <row ht="30" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>566</v>
+        <v>626</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -3704,10 +4649,10 @@
     </row>
     <row ht="30" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>567</v>
+        <v>627</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -3771,10 +4716,10 @@
     </row>
     <row ht="30" r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>568</v>
+        <v>628</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -3838,10 +4783,10 @@
     </row>
     <row ht="30" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>569</v>
+        <v>629</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -3905,10 +4850,10 @@
     </row>
     <row ht="30" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>570</v>
+        <v>630</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -3972,10 +4917,10 @@
     </row>
     <row ht="30" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>571</v>
+        <v>631</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -4039,10 +4984,10 @@
     </row>
     <row ht="30" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>572</v>
+        <v>632</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -4109,7 +5054,7 @@
         <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>573</v>
+        <v>633</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -4173,10 +5118,10 @@
     </row>
     <row ht="30" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>574</v>
+        <v>634</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -4240,10 +5185,10 @@
     </row>
     <row ht="30" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>575</v>
+        <v>635</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -4307,10 +5252,10 @@
     </row>
     <row ht="30" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>576</v>
+        <v>636</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -4377,7 +5322,7 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>577</v>
+        <v>637</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -4441,10 +5386,10 @@
     </row>
     <row ht="30" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>578</v>
+        <v>638</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -4508,10 +5453,10 @@
     </row>
     <row ht="30" r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>579</v>
+        <v>639</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -4578,7 +5523,7 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>580</v>
+        <v>640</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -4645,7 +5590,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>581</v>
+        <v>641</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -4709,10 +5654,10 @@
     </row>
     <row ht="30" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>582</v>
+        <v>642</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -4776,10 +5721,10 @@
     </row>
     <row ht="30" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>583</v>
+        <v>643</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -4846,7 +5791,7 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>584</v>
+        <v>644</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -4910,10 +5855,10 @@
     </row>
     <row ht="30" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>585</v>
+        <v>645</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -4977,10 +5922,10 @@
     </row>
     <row ht="30" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>586</v>
+        <v>646</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -5047,7 +5992,7 @@
         <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>587</v>
+        <v>647</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -5114,7 +6059,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>588</v>
+        <v>648</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -5181,7 +6126,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>497</v>
+        <v>649</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -5248,7 +6193,7 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>498</v>
+        <v>650</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -5312,10 +6257,10 @@
     </row>
     <row ht="30" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>499</v>
+        <v>651</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -5382,7 +6327,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>500</v>
+        <v>652</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -5449,7 +6394,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>501</v>
+        <v>653</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -5513,10 +6458,10 @@
     </row>
     <row ht="30" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>502</v>
+        <v>654</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -5580,10 +6525,10 @@
     </row>
     <row ht="45" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>503</v>
+        <v>655</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>109</v>
@@ -5647,10 +6592,10 @@
     </row>
     <row ht="45" r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>504</v>
+        <v>656</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>104</v>
@@ -5714,10 +6659,10 @@
     </row>
     <row ht="45" r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>505</v>
+        <v>657</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>110</v>
@@ -5908,10 +6853,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>352</v>
+        <v>850</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -5976,10 +6921,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>851</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -6044,10 +6989,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>354</v>
+        <v>852</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -6112,10 +7057,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>355</v>
+        <v>853</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -6180,10 +7125,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>356</v>
+        <v>854</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -6248,10 +7193,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>855</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -6316,10 +7261,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
+        <v>856</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -6384,10 +7329,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>359</v>
+        <v>857</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -6452,10 +7397,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>360</v>
+        <v>858</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -6770,10 +7715,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>429</v>
+        <v>859</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -6838,10 +7783,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>860</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -6909,7 +7854,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>431</v>
+        <v>861</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -6977,7 +7922,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>432</v>
+        <v>862</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -7045,7 +7990,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>863</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -7113,7 +8058,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>434</v>
+        <v>864</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -7181,7 +8126,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>435</v>
+        <v>865</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -7249,7 +8194,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>436</v>
+        <v>866</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -7317,7 +8262,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>867</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -7632,10 +8577,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>868</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -7700,10 +8645,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>869</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -7768,10 +8713,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>870</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -7836,10 +8781,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>871</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -7904,10 +8849,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>374</v>
+        <v>872</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -7972,10 +8917,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>873</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -8040,10 +8985,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>874</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -8108,10 +9053,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>875</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -8176,10 +9121,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>876</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -8499,10 +9444,10 @@
     </row>
     <row ht="60" r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>589</v>
+        <v>877</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -8567,10 +9512,10 @@
     </row>
     <row ht="60" r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>878</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -8635,10 +9580,10 @@
     </row>
     <row ht="60" r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>591</v>
+        <v>879</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -8703,10 +9648,10 @@
     </row>
     <row ht="60" r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>592</v>
+        <v>880</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -8774,7 +9719,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>593</v>
+        <v>881</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -8842,7 +9787,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>594</v>
+        <v>882</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -8907,10 +9852,10 @@
     </row>
     <row ht="60" r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>595</v>
+        <v>883</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -8978,7 +9923,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>596</v>
+        <v>884</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -9043,10 +9988,10 @@
     </row>
     <row ht="60" r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>597</v>
+        <v>885</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -9365,10 +10310,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>598</v>
+        <v>886</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -9433,10 +10378,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>599</v>
+        <v>887</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -9501,10 +10446,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>600</v>
+        <v>888</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -9569,10 +10514,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>601</v>
+        <v>889</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -9640,7 +10585,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>602</v>
+        <v>890</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -9708,7 +10653,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>603</v>
+        <v>891</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -9773,10 +10718,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>604</v>
+        <v>892</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -9841,10 +10786,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>605</v>
+        <v>893</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -9912,7 +10857,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>606</v>
+        <v>894</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -10227,10 +11172,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>895</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -10295,10 +11240,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>447</v>
+        <v>896</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -10366,7 +11311,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>448</v>
+        <v>897</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -10434,7 +11379,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>449</v>
+        <v>898</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -10502,7 +11447,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>450</v>
+        <v>899</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -10570,7 +11515,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>451</v>
+        <v>900</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -10638,7 +11583,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>452</v>
+        <v>901</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -10706,7 +11651,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>453</v>
+        <v>902</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -10774,7 +11719,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>454</v>
+        <v>903</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -11089,10 +12034,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>904</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -11157,10 +12102,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>407</v>
+        <v>905</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -11225,10 +12170,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>408</v>
+        <v>906</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -11293,10 +12238,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>409</v>
+        <v>907</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -11361,10 +12306,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>410</v>
+        <v>908</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -11429,10 +12374,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>411</v>
+        <v>909</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -11497,10 +12442,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>412</v>
+        <v>910</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -11565,10 +12510,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>413</v>
+        <v>911</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -11633,10 +12578,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>414</v>
+        <v>912</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -11951,7 +12896,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>506</v>
+        <v>658</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -12018,7 +12963,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>659</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -12085,7 +13030,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>508</v>
+        <v>660</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -12152,7 +13097,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>509</v>
+        <v>661</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -12219,7 +13164,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>510</v>
+        <v>662</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -12286,7 +13231,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>511</v>
+        <v>663</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -12350,10 +13295,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>512</v>
+        <v>664</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -12420,7 +13365,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>513</v>
+        <v>665</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -12484,10 +13429,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>514</v>
+        <v>666</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -12551,10 +13496,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>515</v>
+        <v>667</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -12618,10 +13563,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>516</v>
+        <v>668</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -12688,7 +13633,7 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>517</v>
+        <v>669</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -12755,7 +13700,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>518</v>
+        <v>670</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -12822,7 +13767,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>519</v>
+        <v>671</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -12889,7 +13834,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>520</v>
+        <v>672</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -12956,7 +13901,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>521</v>
+        <v>673</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -13020,10 +13965,10 @@
     </row>
     <row ht="75" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>522</v>
+        <v>674</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -13090,7 +14035,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>523</v>
+        <v>675</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -13157,7 +14102,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>524</v>
+        <v>676</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -13221,10 +14166,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>525</v>
+        <v>677</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -13291,7 +14236,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>526</v>
+        <v>678</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -13358,7 +14303,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>527</v>
+        <v>679</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -13425,7 +14370,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>528</v>
+        <v>680</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -13492,7 +14437,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>529</v>
+        <v>681</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -13559,7 +14504,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>530</v>
+        <v>682</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -13623,10 +14568,10 @@
     </row>
     <row ht="75" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>531</v>
+        <v>683</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -13693,7 +14638,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>532</v>
+        <v>684</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -13757,10 +14702,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>533</v>
+        <v>685</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -13824,10 +14769,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>534</v>
+        <v>686</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -13894,7 +14839,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>535</v>
+        <v>687</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -13961,7 +14906,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>536</v>
+        <v>688</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -14028,7 +14973,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>537</v>
+        <v>689</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -14095,7 +15040,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>538</v>
+        <v>690</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -14162,7 +15107,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>539</v>
+        <v>691</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -14226,10 +15171,10 @@
     </row>
     <row ht="75" r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>540</v>
+        <v>692</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -14296,7 +15241,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>541</v>
+        <v>693</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -14360,10 +15305,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>542</v>
+        <v>694</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -14427,10 +15372,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>543</v>
+        <v>695</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -14494,10 +15439,10 @@
     </row>
     <row ht="75" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>544</v>
+        <v>696</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -14564,7 +15509,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>545</v>
+        <v>697</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -14628,10 +15573,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>546</v>
+        <v>698</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -14695,10 +15640,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>699</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -14765,7 +15710,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>212</v>
+        <v>700</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -14829,10 +15774,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>213</v>
+        <v>701</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -14899,7 +15844,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>214</v>
+        <v>702</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -14966,7 +15911,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>703</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -15030,10 +15975,10 @@
     </row>
     <row ht="75" r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>704</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -15097,10 +16042,10 @@
     </row>
     <row ht="75" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>705</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -15164,10 +16109,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>706</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -15361,7 +16306,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>707</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -15425,10 +16370,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>708</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -15495,7 +16440,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>709</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -15562,7 +16507,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>710</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -15626,10 +16571,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>711</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -15693,10 +16638,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>712</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -15763,7 +16708,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>713</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -15830,7 +16775,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>714</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -15897,7 +16842,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>715</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -15961,10 +16906,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>716</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -16028,10 +16973,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>717</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -16095,10 +17040,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>718</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -16165,7 +17110,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>719</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -16232,7 +17177,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>720</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -16299,7 +17244,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>721</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -16366,7 +17311,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>722</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -16433,7 +17378,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>723</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -16500,7 +17445,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>724</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -16564,10 +17509,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>725</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -16631,10 +17576,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>726</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -16698,10 +17643,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>239</v>
+        <v>727</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -16768,7 +17713,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>240</v>
+        <v>728</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -16835,7 +17780,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>729</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -16902,7 +17847,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>730</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -16966,10 +17911,10 @@
     </row>
     <row ht="75" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>731</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -17036,7 +17981,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>732</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -17103,7 +18048,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>245</v>
+        <v>733</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -17167,10 +18112,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>246</v>
+        <v>734</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -17234,10 +18179,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>735</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -17304,7 +18249,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>736</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -17368,10 +18313,10 @@
     </row>
     <row ht="75" r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>249</v>
+        <v>737</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -17435,10 +18380,10 @@
     </row>
     <row ht="75" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>738</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -17505,7 +18450,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>251</v>
+        <v>739</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -17569,10 +18514,10 @@
     </row>
     <row ht="75" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>740</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -17639,7 +18584,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>741</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -17703,10 +18648,10 @@
     </row>
     <row ht="75" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>742</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -17770,10 +18715,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>255</v>
+        <v>743</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -17840,7 +18785,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>256</v>
+        <v>744</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -17907,7 +18852,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>257</v>
+        <v>745</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -17971,10 +18916,10 @@
     </row>
     <row ht="75" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>258</v>
+        <v>746</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -18041,7 +18986,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>259</v>
+        <v>747</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -18105,10 +19050,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>260</v>
+        <v>748</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -18175,7 +19120,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>261</v>
+        <v>749</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -18239,10 +19184,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>750</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -18309,7 +19254,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>751</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -18376,7 +19321,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>752</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -18443,7 +19388,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>753</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -18510,7 +19455,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>754</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -18577,7 +19522,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>755</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -18770,7 +19715,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>756</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -18834,10 +19779,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>757</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -18901,10 +19846,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>758</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -18968,10 +19913,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>759</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -19035,10 +19980,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>760</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -19102,10 +20047,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>761</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -19169,10 +20114,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
+        <v>762</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -19236,10 +20181,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>763</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -19303,10 +20248,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>764</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -19370,10 +20315,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>765</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -19437,10 +20382,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>278</v>
+        <v>766</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -19504,10 +20449,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>767</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -19571,10 +20516,10 @@
     </row>
     <row ht="75" r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>280</v>
+        <v>768</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -19638,10 +20583,10 @@
     </row>
     <row ht="75" r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>769</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -19705,10 +20650,10 @@
     </row>
     <row ht="75" r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>282</v>
+        <v>770</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -19772,10 +20717,10 @@
     </row>
     <row ht="75" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>283</v>
+        <v>771</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -19839,10 +20784,10 @@
     </row>
     <row ht="75" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>772</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -19906,10 +20851,10 @@
     </row>
     <row ht="75" r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>285</v>
+        <v>773</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -19973,10 +20918,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>286</v>
+        <v>774</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -20040,10 +20985,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>287</v>
+        <v>775</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -20107,10 +21052,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>776</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -20174,10 +21119,10 @@
     </row>
     <row ht="75" r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>289</v>
+        <v>777</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -20241,10 +21186,10 @@
     </row>
     <row ht="75" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>290</v>
+        <v>778</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -20308,10 +21253,10 @@
     </row>
     <row ht="75" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>291</v>
+        <v>779</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -20375,10 +21320,10 @@
     </row>
     <row ht="75" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>780</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -20442,10 +21387,10 @@
     </row>
     <row ht="75" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>781</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -20509,10 +21454,10 @@
     </row>
     <row ht="75" r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>294</v>
+        <v>782</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -20576,10 +21521,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>295</v>
+        <v>783</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -20643,10 +21588,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>784</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -20710,10 +21655,10 @@
     </row>
     <row ht="75" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>297</v>
+        <v>785</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -20777,10 +21722,10 @@
     </row>
     <row ht="75" r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>298</v>
+        <v>786</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -20844,10 +21789,10 @@
     </row>
     <row ht="75" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>299</v>
+        <v>787</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -20911,10 +21856,10 @@
     </row>
     <row ht="75" r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>300</v>
+        <v>788</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -20978,10 +21923,10 @@
     </row>
     <row ht="75" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>301</v>
+        <v>789</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -21045,10 +21990,10 @@
     </row>
     <row ht="75" r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>302</v>
+        <v>790</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -21112,10 +22057,10 @@
     </row>
     <row ht="75" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>303</v>
+        <v>791</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -21179,10 +22124,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>304</v>
+        <v>792</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -21246,10 +22191,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>305</v>
+        <v>793</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -21313,10 +22258,10 @@
     </row>
     <row ht="75" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>794</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -21380,10 +22325,10 @@
     </row>
     <row ht="75" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>307</v>
+        <v>795</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -21447,10 +22392,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>796</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -21514,10 +22459,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>797</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -21581,10 +22526,10 @@
     </row>
     <row ht="75" r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>310</v>
+        <v>798</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -21648,10 +22593,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>311</v>
+        <v>799</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -21715,10 +22660,10 @@
     </row>
     <row ht="75" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>312</v>
+        <v>800</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -21782,10 +22727,10 @@
     </row>
     <row ht="75" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>313</v>
+        <v>801</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -21849,10 +22794,10 @@
     </row>
     <row ht="75" r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>314</v>
+        <v>802</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -21916,10 +22861,10 @@
     </row>
     <row ht="75" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>315</v>
+        <v>803</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -21983,10 +22928,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>316</v>
+        <v>804</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -22180,10 +23125,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>805</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -22247,10 +23192,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>806</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -22314,10 +23259,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>807</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -22381,10 +23326,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>808</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -22448,10 +23393,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>809</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -22515,10 +23460,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>322</v>
+        <v>810</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -22582,10 +23527,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>811</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -22649,10 +23594,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>324</v>
+        <v>812</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -22716,10 +23661,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>325</v>
+        <v>813</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -23035,7 +23980,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>913</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -23102,7 +24047,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>914</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -23169,7 +24114,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>915</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -23233,10 +24178,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>916</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -23303,7 +24248,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>330</v>
+        <v>917</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -23367,10 +24312,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>918</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -23434,10 +24379,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>919</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -23501,10 +24446,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>333</v>
+        <v>920</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -23571,7 +24516,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>334</v>
+        <v>921</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -23885,10 +24830,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>823</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -23952,10 +24897,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>416</v>
+        <v>824</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -24022,7 +24967,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>417</v>
+        <v>825</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -24089,7 +25034,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>826</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -24156,7 +25101,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>827</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -24223,7 +25168,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>828</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -24290,7 +25235,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>829</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -24357,7 +25302,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>830</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -24424,7 +25369,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>423</v>
+        <v>831</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -24738,10 +25683,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>335</v>
+        <v>832</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -24805,10 +25750,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>336</v>
+        <v>833</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -24872,10 +25817,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
+        <v>834</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -24939,10 +25884,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>835</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -25006,10 +25951,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>428</v>
+        <v>836</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -25073,10 +26018,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>837</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -25140,10 +26085,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>838</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -25207,10 +26152,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>839</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -25274,10 +26219,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>342</v>
+        <v>840</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -25592,10 +26537,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>841</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -25660,10 +26605,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>344</v>
+        <v>842</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -25728,10 +26673,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>843</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -25796,10 +26741,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>346</v>
+        <v>844</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -25864,10 +26809,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>845</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -25932,10 +26877,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>348</v>
+        <v>846</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -26000,10 +26945,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>349</v>
+        <v>847</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -26068,10 +27013,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>848</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -26136,10 +27081,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>351</v>
+        <v>849</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Testing Object Repo for BWP
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/DisplayCFData.xlsx
+++ b/KatalonData/IWPTestData/DisplayCFData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5932" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7192" uniqueCount="922">
   <si>
     <t>Result</t>
   </si>
@@ -1861,6 +1861,951 @@
   </si>
   <si>
     <t>Tue Jul 29 21:03:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:30:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:31:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:32:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:33:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:34:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:35:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:35:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:36:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:37:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:38:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:40:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:40:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:42:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:43:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:44:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:45:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:45:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:47:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:48:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:49:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:49:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:50:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:51:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:52:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:53:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:54:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:55:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 22:59:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:00:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:01:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:02:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:03:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:04:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:05:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:06:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:08:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:09:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:09:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:11:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:12:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:13:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:14:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:15:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:16:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:17:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:18:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:19:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:20:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:22:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:23:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:24:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:26:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:27:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:27:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:28:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:29:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:30:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:31:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:32:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:33:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:34:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:36:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:37:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:38:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:39:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:40:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:40:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:41:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:42:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:43:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:44:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:47:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:48:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:48:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:49:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:50:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:51:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:52:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:53:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:55:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:56:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:57:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:58:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 23:59:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:00:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:00:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:02:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:03:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:04:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:05:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:07:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:08:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:09:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:10:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:11:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:12:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:13:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:14:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:15:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:17:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:18:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:19:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:21:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:21:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:22:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:24:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:25:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:26:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:27:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:27:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:29:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:30:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:32:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:33:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:34:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:35:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:36:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:36:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:37:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:41:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:42:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:44:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:45:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:46:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:47:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:48:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:49:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:50:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:51:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:53:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:53:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:55:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:56:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:57:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 00:59:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:00:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:01:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:03:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:03:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:04:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:06:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:07:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:08:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:09:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:10:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:11:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:12:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:13:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:14:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:15:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:16:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:17:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:18:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:19:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:20:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:21:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:22:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:23:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:24:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:25:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:26:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:27:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:28:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:29:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:30:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:31:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:32:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:33:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:34:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:35:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:36:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:37:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:38:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:39:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:40:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:41:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:42:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:43:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:44:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:45:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:46:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:47:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:48:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:49:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:50:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:51:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:52:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:53:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:54:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:55:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:56:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:57:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:58:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 01:59:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:00:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:01:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:02:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 02:03:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:08:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:10:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:11:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:12:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:14:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:16:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:17:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:19:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 26 20:21:09 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -2364,10 +3309,10 @@
     </row>
     <row ht="30" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
+        <v>607</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -2431,10 +3376,10 @@
     </row>
     <row ht="30" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>548</v>
+        <v>608</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -2498,10 +3443,10 @@
     </row>
     <row ht="30" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>549</v>
+        <v>609</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -2565,10 +3510,10 @@
     </row>
     <row ht="30" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>550</v>
+        <v>610</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -2632,10 +3577,10 @@
     </row>
     <row ht="30" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>551</v>
+        <v>611</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -2699,10 +3644,10 @@
     </row>
     <row ht="30" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>552</v>
+        <v>612</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -2766,10 +3711,10 @@
     </row>
     <row ht="30" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>553</v>
+        <v>613</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -2833,10 +3778,10 @@
     </row>
     <row ht="30" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -2900,10 +3845,10 @@
     </row>
     <row ht="30" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>555</v>
+        <v>615</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2970,7 +3915,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>556</v>
+        <v>616</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -3034,10 +3979,10 @@
     </row>
     <row ht="30" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>557</v>
+        <v>617</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -3104,7 +4049,7 @@
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>558</v>
+        <v>618</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -3168,10 +4113,10 @@
     </row>
     <row ht="30" r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>559</v>
+        <v>619</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -3235,10 +4180,10 @@
     </row>
     <row ht="30" r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>560</v>
+        <v>620</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -3302,10 +4247,10 @@
     </row>
     <row ht="30" r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>561</v>
+        <v>621</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -3369,10 +4314,10 @@
     </row>
     <row ht="30" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>562</v>
+        <v>622</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -3439,7 +4384,7 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>563</v>
+        <v>623</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -3503,10 +4448,10 @@
     </row>
     <row ht="30" r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>564</v>
+        <v>624</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -3570,10 +4515,10 @@
     </row>
     <row ht="30" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>565</v>
+        <v>625</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -3637,10 +4582,10 @@
     </row>
     <row ht="30" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>566</v>
+        <v>626</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -3704,10 +4649,10 @@
     </row>
     <row ht="30" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>567</v>
+        <v>627</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -3771,10 +4716,10 @@
     </row>
     <row ht="30" r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>568</v>
+        <v>628</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -3838,10 +4783,10 @@
     </row>
     <row ht="30" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>569</v>
+        <v>629</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -3905,10 +4850,10 @@
     </row>
     <row ht="30" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>570</v>
+        <v>630</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -3972,10 +4917,10 @@
     </row>
     <row ht="30" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>571</v>
+        <v>631</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -4039,10 +4984,10 @@
     </row>
     <row ht="30" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>572</v>
+        <v>632</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -4109,7 +5054,7 @@
         <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>573</v>
+        <v>633</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -4173,10 +5118,10 @@
     </row>
     <row ht="30" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>574</v>
+        <v>634</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -4240,10 +5185,10 @@
     </row>
     <row ht="30" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>575</v>
+        <v>635</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -4307,10 +5252,10 @@
     </row>
     <row ht="30" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>576</v>
+        <v>636</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -4377,7 +5322,7 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>577</v>
+        <v>637</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -4441,10 +5386,10 @@
     </row>
     <row ht="30" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>578</v>
+        <v>638</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -4508,10 +5453,10 @@
     </row>
     <row ht="30" r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>579</v>
+        <v>639</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -4578,7 +5523,7 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>580</v>
+        <v>640</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -4645,7 +5590,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>581</v>
+        <v>641</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -4709,10 +5654,10 @@
     </row>
     <row ht="30" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>582</v>
+        <v>642</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -4776,10 +5721,10 @@
     </row>
     <row ht="30" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>583</v>
+        <v>643</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -4846,7 +5791,7 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>584</v>
+        <v>644</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -4910,10 +5855,10 @@
     </row>
     <row ht="30" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>585</v>
+        <v>645</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -4977,10 +5922,10 @@
     </row>
     <row ht="30" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>586</v>
+        <v>646</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -5047,7 +5992,7 @@
         <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>587</v>
+        <v>647</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -5114,7 +6059,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>588</v>
+        <v>648</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -5181,7 +6126,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>497</v>
+        <v>649</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -5248,7 +6193,7 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>498</v>
+        <v>650</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -5312,10 +6257,10 @@
     </row>
     <row ht="30" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>499</v>
+        <v>651</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -5382,7 +6327,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>500</v>
+        <v>652</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -5449,7 +6394,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>501</v>
+        <v>653</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -5513,10 +6458,10 @@
     </row>
     <row ht="30" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>502</v>
+        <v>654</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -5580,10 +6525,10 @@
     </row>
     <row ht="45" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>503</v>
+        <v>655</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>109</v>
@@ -5647,10 +6592,10 @@
     </row>
     <row ht="45" r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>504</v>
+        <v>656</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>104</v>
@@ -5714,10 +6659,10 @@
     </row>
     <row ht="45" r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>505</v>
+        <v>657</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>110</v>
@@ -5908,10 +6853,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>352</v>
+        <v>850</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -5976,10 +6921,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>851</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -6044,10 +6989,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>354</v>
+        <v>852</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -6112,10 +7057,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>355</v>
+        <v>853</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -6180,10 +7125,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>356</v>
+        <v>854</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -6248,10 +7193,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>855</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -6316,10 +7261,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
+        <v>856</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -6384,10 +7329,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>359</v>
+        <v>857</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -6452,10 +7397,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>360</v>
+        <v>858</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -6770,10 +7715,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>429</v>
+        <v>859</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -6838,10 +7783,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>860</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -6909,7 +7854,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>431</v>
+        <v>861</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -6977,7 +7922,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>432</v>
+        <v>862</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -7045,7 +7990,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>863</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -7113,7 +8058,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>434</v>
+        <v>864</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -7181,7 +8126,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>435</v>
+        <v>865</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -7249,7 +8194,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>436</v>
+        <v>866</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -7317,7 +8262,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>867</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -7632,10 +8577,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>868</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -7700,10 +8645,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>869</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -7768,10 +8713,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>870</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -7836,10 +8781,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>871</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -7904,10 +8849,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>374</v>
+        <v>872</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -7972,10 +8917,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>873</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -8040,10 +8985,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>874</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -8108,10 +9053,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>875</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -8176,10 +9121,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>876</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -8499,10 +9444,10 @@
     </row>
     <row ht="60" r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>589</v>
+        <v>877</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -8567,10 +9512,10 @@
     </row>
     <row ht="60" r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>878</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -8635,10 +9580,10 @@
     </row>
     <row ht="60" r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>591</v>
+        <v>879</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -8703,10 +9648,10 @@
     </row>
     <row ht="60" r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>592</v>
+        <v>880</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -8774,7 +9719,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>593</v>
+        <v>881</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -8842,7 +9787,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>594</v>
+        <v>882</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -8907,10 +9852,10 @@
     </row>
     <row ht="60" r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>595</v>
+        <v>883</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -8978,7 +9923,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>596</v>
+        <v>884</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -9043,10 +9988,10 @@
     </row>
     <row ht="60" r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>597</v>
+        <v>885</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -9365,10 +10310,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>598</v>
+        <v>886</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -9433,10 +10378,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>599</v>
+        <v>887</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -9501,10 +10446,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>600</v>
+        <v>888</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -9569,10 +10514,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>601</v>
+        <v>889</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -9640,7 +10585,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>602</v>
+        <v>890</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -9708,7 +10653,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>603</v>
+        <v>891</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -9773,10 +10718,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>604</v>
+        <v>892</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -9841,10 +10786,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>605</v>
+        <v>893</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -9912,7 +10857,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>606</v>
+        <v>894</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -10227,10 +11172,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>895</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -10295,10 +11240,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>447</v>
+        <v>896</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -10366,7 +11311,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>448</v>
+        <v>897</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -10434,7 +11379,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>449</v>
+        <v>898</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -10502,7 +11447,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>450</v>
+        <v>899</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -10570,7 +11515,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>451</v>
+        <v>900</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -10638,7 +11583,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>452</v>
+        <v>901</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -10706,7 +11651,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>453</v>
+        <v>902</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -10774,7 +11719,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>454</v>
+        <v>903</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -11089,10 +12034,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>904</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -11157,10 +12102,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>407</v>
+        <v>905</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -11225,10 +12170,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>408</v>
+        <v>906</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -11293,10 +12238,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>409</v>
+        <v>907</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -11361,10 +12306,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>410</v>
+        <v>908</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -11429,10 +12374,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>411</v>
+        <v>909</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -11497,10 +12442,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>412</v>
+        <v>910</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -11565,10 +12510,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>413</v>
+        <v>911</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -11633,10 +12578,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>414</v>
+        <v>912</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -11951,7 +12896,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>506</v>
+        <v>658</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -12018,7 +12963,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>659</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -12085,7 +13030,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>508</v>
+        <v>660</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -12152,7 +13097,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>509</v>
+        <v>661</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -12219,7 +13164,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>510</v>
+        <v>662</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -12286,7 +13231,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>511</v>
+        <v>663</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -12350,10 +13295,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>512</v>
+        <v>664</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -12420,7 +13365,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>513</v>
+        <v>665</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -12484,10 +13429,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>514</v>
+        <v>666</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -12551,10 +13496,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>515</v>
+        <v>667</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -12618,10 +13563,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>516</v>
+        <v>668</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -12688,7 +13633,7 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>517</v>
+        <v>669</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -12755,7 +13700,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>518</v>
+        <v>670</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -12822,7 +13767,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>519</v>
+        <v>671</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -12889,7 +13834,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>520</v>
+        <v>672</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -12956,7 +13901,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>521</v>
+        <v>673</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -13020,10 +13965,10 @@
     </row>
     <row ht="75" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>522</v>
+        <v>674</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -13090,7 +14035,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>523</v>
+        <v>675</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -13157,7 +14102,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>524</v>
+        <v>676</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -13221,10 +14166,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>525</v>
+        <v>677</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -13291,7 +14236,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>526</v>
+        <v>678</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -13358,7 +14303,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>527</v>
+        <v>679</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -13425,7 +14370,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>528</v>
+        <v>680</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -13492,7 +14437,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>529</v>
+        <v>681</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -13559,7 +14504,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>530</v>
+        <v>682</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -13623,10 +14568,10 @@
     </row>
     <row ht="75" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>531</v>
+        <v>683</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -13693,7 +14638,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>532</v>
+        <v>684</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -13757,10 +14702,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>533</v>
+        <v>685</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -13824,10 +14769,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>534</v>
+        <v>686</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -13894,7 +14839,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>535</v>
+        <v>687</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -13961,7 +14906,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>536</v>
+        <v>688</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -14028,7 +14973,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>537</v>
+        <v>689</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -14095,7 +15040,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>538</v>
+        <v>690</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -14162,7 +15107,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>539</v>
+        <v>691</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -14226,10 +15171,10 @@
     </row>
     <row ht="75" r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>540</v>
+        <v>692</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -14296,7 +15241,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>541</v>
+        <v>693</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -14360,10 +15305,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>542</v>
+        <v>694</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -14427,10 +15372,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>543</v>
+        <v>695</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -14494,10 +15439,10 @@
     </row>
     <row ht="75" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>544</v>
+        <v>696</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -14564,7 +15509,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>545</v>
+        <v>697</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -14628,10 +15573,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>546</v>
+        <v>698</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -14695,10 +15640,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>699</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -14765,7 +15710,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>212</v>
+        <v>700</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -14829,10 +15774,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>213</v>
+        <v>701</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -14899,7 +15844,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>214</v>
+        <v>702</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -14966,7 +15911,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>703</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -15030,10 +15975,10 @@
     </row>
     <row ht="75" r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>704</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -15097,10 +16042,10 @@
     </row>
     <row ht="75" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>705</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -15164,10 +16109,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>706</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -15361,7 +16306,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>707</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -15425,10 +16370,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>708</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -15495,7 +16440,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>709</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -15562,7 +16507,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>710</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -15626,10 +16571,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>711</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -15693,10 +16638,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>712</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -15763,7 +16708,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>713</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -15830,7 +16775,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>714</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -15897,7 +16842,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>715</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -15961,10 +16906,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>716</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -16028,10 +16973,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>717</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -16095,10 +17040,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>718</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -16165,7 +17110,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>719</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -16232,7 +17177,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>720</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -16299,7 +17244,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>721</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -16366,7 +17311,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>722</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -16433,7 +17378,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>723</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -16500,7 +17445,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>724</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -16564,10 +17509,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>725</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -16631,10 +17576,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>726</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -16698,10 +17643,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>239</v>
+        <v>727</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -16768,7 +17713,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>240</v>
+        <v>728</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -16835,7 +17780,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>729</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -16902,7 +17847,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>730</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -16966,10 +17911,10 @@
     </row>
     <row ht="75" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>731</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -17036,7 +17981,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>732</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -17103,7 +18048,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>245</v>
+        <v>733</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -17167,10 +18112,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>246</v>
+        <v>734</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -17234,10 +18179,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>735</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -17304,7 +18249,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>736</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -17368,10 +18313,10 @@
     </row>
     <row ht="75" r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>249</v>
+        <v>737</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -17435,10 +18380,10 @@
     </row>
     <row ht="75" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>738</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -17505,7 +18450,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>251</v>
+        <v>739</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -17569,10 +18514,10 @@
     </row>
     <row ht="75" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>740</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -17639,7 +18584,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>741</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -17703,10 +18648,10 @@
     </row>
     <row ht="75" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>742</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -17770,10 +18715,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>255</v>
+        <v>743</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -17840,7 +18785,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>256</v>
+        <v>744</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -17907,7 +18852,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>257</v>
+        <v>745</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -17971,10 +18916,10 @@
     </row>
     <row ht="75" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>258</v>
+        <v>746</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -18041,7 +18986,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>259</v>
+        <v>747</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -18105,10 +19050,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>260</v>
+        <v>748</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -18175,7 +19120,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>261</v>
+        <v>749</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -18239,10 +19184,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>750</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -18309,7 +19254,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>751</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -18376,7 +19321,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>752</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -18443,7 +19388,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>753</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -18510,7 +19455,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>754</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -18577,7 +19522,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>755</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -18770,7 +19715,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>756</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -18834,10 +19779,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>757</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -18901,10 +19846,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>758</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -18968,10 +19913,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>759</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -19035,10 +19980,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>760</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -19102,10 +20047,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>761</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -19169,10 +20114,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
+        <v>762</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -19236,10 +20181,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>763</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -19303,10 +20248,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>764</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -19370,10 +20315,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>765</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -19437,10 +20382,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>278</v>
+        <v>766</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -19504,10 +20449,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>767</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -19571,10 +20516,10 @@
     </row>
     <row ht="75" r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>280</v>
+        <v>768</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -19638,10 +20583,10 @@
     </row>
     <row ht="75" r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>769</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -19705,10 +20650,10 @@
     </row>
     <row ht="75" r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>282</v>
+        <v>770</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -19772,10 +20717,10 @@
     </row>
     <row ht="75" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>283</v>
+        <v>771</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -19839,10 +20784,10 @@
     </row>
     <row ht="75" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>772</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -19906,10 +20851,10 @@
     </row>
     <row ht="75" r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>285</v>
+        <v>773</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -19973,10 +20918,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>286</v>
+        <v>774</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -20040,10 +20985,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>287</v>
+        <v>775</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -20107,10 +21052,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>776</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -20174,10 +21119,10 @@
     </row>
     <row ht="75" r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>289</v>
+        <v>777</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -20241,10 +21186,10 @@
     </row>
     <row ht="75" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>290</v>
+        <v>778</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -20308,10 +21253,10 @@
     </row>
     <row ht="75" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>291</v>
+        <v>779</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -20375,10 +21320,10 @@
     </row>
     <row ht="75" r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>780</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -20442,10 +21387,10 @@
     </row>
     <row ht="75" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>781</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -20509,10 +21454,10 @@
     </row>
     <row ht="75" r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>294</v>
+        <v>782</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -20576,10 +21521,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>295</v>
+        <v>783</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -20643,10 +21588,10 @@
     </row>
     <row ht="75" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>784</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -20710,10 +21655,10 @@
     </row>
     <row ht="75" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>297</v>
+        <v>785</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -20777,10 +21722,10 @@
     </row>
     <row ht="75" r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>298</v>
+        <v>786</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -20844,10 +21789,10 @@
     </row>
     <row ht="75" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>299</v>
+        <v>787</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -20911,10 +21856,10 @@
     </row>
     <row ht="75" r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>300</v>
+        <v>788</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -20978,10 +21923,10 @@
     </row>
     <row ht="75" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>301</v>
+        <v>789</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -21045,10 +21990,10 @@
     </row>
     <row ht="75" r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>302</v>
+        <v>790</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -21112,10 +22057,10 @@
     </row>
     <row ht="75" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>303</v>
+        <v>791</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -21179,10 +22124,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>304</v>
+        <v>792</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -21246,10 +22191,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>305</v>
+        <v>793</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -21313,10 +22258,10 @@
     </row>
     <row ht="75" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>794</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -21380,10 +22325,10 @@
     </row>
     <row ht="75" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>307</v>
+        <v>795</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -21447,10 +22392,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>796</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -21514,10 +22459,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>797</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -21581,10 +22526,10 @@
     </row>
     <row ht="75" r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>310</v>
+        <v>798</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -21648,10 +22593,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>311</v>
+        <v>799</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -21715,10 +22660,10 @@
     </row>
     <row ht="75" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>312</v>
+        <v>800</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -21782,10 +22727,10 @@
     </row>
     <row ht="75" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>313</v>
+        <v>801</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -21849,10 +22794,10 @@
     </row>
     <row ht="75" r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>314</v>
+        <v>802</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -21916,10 +22861,10 @@
     </row>
     <row ht="75" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>315</v>
+        <v>803</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -21983,10 +22928,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>316</v>
+        <v>804</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -22180,10 +23125,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>805</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -22247,10 +23192,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>806</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -22314,10 +23259,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>807</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -22381,10 +23326,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>808</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -22448,10 +23393,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>809</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -22515,10 +23460,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>322</v>
+        <v>810</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -22582,10 +23527,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>811</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -22649,10 +23594,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>324</v>
+        <v>812</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -22716,10 +23661,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>325</v>
+        <v>813</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -23035,7 +23980,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>913</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -23102,7 +24047,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>914</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -23169,7 +24114,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>915</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -23233,10 +24178,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>916</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -23303,7 +24248,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>330</v>
+        <v>917</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -23367,10 +24312,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>918</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -23434,10 +24379,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>919</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -23501,10 +24446,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>333</v>
+        <v>920</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -23571,7 +24516,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>334</v>
+        <v>921</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -23885,10 +24830,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>823</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -23952,10 +24897,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>416</v>
+        <v>824</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -24022,7 +24967,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>417</v>
+        <v>825</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -24089,7 +25034,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>826</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -24156,7 +25101,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>827</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -24223,7 +25168,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>828</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -24290,7 +25235,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>829</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -24357,7 +25302,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>830</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -24424,7 +25369,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>423</v>
+        <v>831</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -24738,10 +25683,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>335</v>
+        <v>832</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -24805,10 +25750,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>336</v>
+        <v>833</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -24872,10 +25817,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
+        <v>834</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -24939,10 +25884,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>835</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -25006,10 +25951,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>428</v>
+        <v>836</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -25073,10 +26018,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>837</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -25140,10 +26085,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>838</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -25207,10 +26152,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>839</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -25274,10 +26219,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>342</v>
+        <v>840</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -25592,10 +26537,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>841</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -25660,10 +26605,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>344</v>
+        <v>842</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -25728,10 +26673,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>843</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -25796,10 +26741,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>346</v>
+        <v>844</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -25864,10 +26809,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>845</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -25932,10 +26877,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>348</v>
+        <v>846</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -26000,10 +26945,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>349</v>
+        <v>847</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -26068,10 +27013,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>848</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -26136,10 +27081,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>351</v>
+        <v>849</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Fix for Display CF
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/DisplayCFData.xlsx
+++ b/KatalonData/IWPTestData/DisplayCFData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9580" uniqueCount="1519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12032" uniqueCount="2132">
   <si>
     <t>Result</t>
   </si>
@@ -4597,6 +4597,1845 @@
   </si>
   <si>
     <t>Tue Sep 02 08:42:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:51:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:53:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:55:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:56:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:58:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 12:59:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:00:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:02:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:03:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:04:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:06:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:07:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:08:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:10:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:11:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:12:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:13:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:15:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:16:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:17:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:18:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:20:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:21:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:22:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:24:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:25:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:26:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:28:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:29:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:30:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:32:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:33:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:34:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:36:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:37:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:38:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:40:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:41:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:43:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:44:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:45:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:46:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:48:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:49:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:50:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:52:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 13:53:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:00:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:02:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:19:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:20:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:22:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:24:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:25:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:27:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:28:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:30:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:31:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:33:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:34:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:36:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:38:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:40:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:41:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:43:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:44:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:46:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:48:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:49:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:51:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:52:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:54:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:55:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:57:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 14:59:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:00:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:02:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:03:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:05:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:06:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:08:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:09:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:11:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:14:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:15:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:17:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:19:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:20:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:22:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:23:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:25:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:26:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:28:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:29:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:30:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:31:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:33:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:34:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:36:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:37:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:39:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:40:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:41:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:43:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:44:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:45:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:47:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:48:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:49:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:51:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:52:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:54:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:56:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:58:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 15:59:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:00:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:01:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:03:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:04:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:06:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:07:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:09:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:10:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:11:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:13:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:14:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:15:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:16:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:18:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:19:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:20:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:22:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:23:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:25:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:26:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:28:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:29:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:30:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:31:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:33:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:34:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:35:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:37:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:38:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:39:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:41:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:42:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:43:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:45:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:49:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:51:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:52:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:54:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:56:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 16:58:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:00:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:01:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:03:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:04:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:06:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:08:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:09:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:11:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:13:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:15:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:17:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:18:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:19:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:21:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:23:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:25:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:27:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:28:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:30:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:31:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:33:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:35:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:36:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:38:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:40:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:42:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:43:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:45:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:46:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:48:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:49:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:51:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:53:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:55:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:57:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:58:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 17:59:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:01:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:03:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:05:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:07:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:09:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:11:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:13:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:14:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:16:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:17:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:19:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:20:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:21:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:23:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:24:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:26:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:28:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:29:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:30:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:32:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:33:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:35:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:36:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:38:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:39:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:41:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:42:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:44:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:46:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:47:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:49:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:50:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:52:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:53:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:55:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:56:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:58:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 18:59:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:01:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:02:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:04:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:05:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:07:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:08:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:09:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:10:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:11:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:12:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:14:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:15:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:17:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:18:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:19:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:20:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:22:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:23:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:24:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:26:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:27:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:29:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:30:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:32:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:33:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:35:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:36:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:38:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:39:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:40:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:41:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:43:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:44:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:45:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:47:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:48:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:49:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:50:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:52:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:53:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:55:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:56:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:57:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 19:59:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:00:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:01:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:02:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:03:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:05:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:06:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:08:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:09:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:10:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:11:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:13:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:14:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:15:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:17:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:18:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:20:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:21:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:23:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:24:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:26:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:27:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:28:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:30:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:31:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:32:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:34:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:35:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:36:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:38:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:39:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:40:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Sep 06 20:41:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:28:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:30:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:32:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:33:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:34:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:36:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:37:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:39:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:40:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:41:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:42:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:44:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:45:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:46:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:48:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:49:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:50:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:52:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:53:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:54:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:56:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:57:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 02:58:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:00:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:01:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:02:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:04:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:05:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:06:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:08:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:09:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:10:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:11:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:13:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:14:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:15:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:17:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:18:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:19:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:21:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:22:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:23:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:25:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:26:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:27:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:29:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:30:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:31:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:32:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:34:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:35:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:37:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:38:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:39:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:40:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:42:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:43:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:44:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:46:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:47:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:49:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:50:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:51:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:52:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:54:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:55:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:56:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:58:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 03:59:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:00:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:01:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:03:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:04:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:05:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:07:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:08:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:09:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:11:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:12:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:13:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:14:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:16:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:18:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:19:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:20:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:22:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:23:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:24:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:26:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:27:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:28:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:30:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:31:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:32:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:34:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:35:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:37:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:38:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:40:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:41:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:43:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:44:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:45:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:47:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:48:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:49:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:50:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:51:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:53:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:54:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:56:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:57:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 04:59:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:00:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:01:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:03:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:04:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:05:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:07:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:08:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:09:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:10:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:12:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:13:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:15:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:16:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:18:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:19:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:20:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:22:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:23:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:24:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:26:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:28:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:29:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:30:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:32:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:33:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:34:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:36:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:37:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:39:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:40:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:41:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:43:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:44:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:45:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:47:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:48:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:49:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:50:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:52:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:54:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:56:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:58:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 05:59:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:01:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:03:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:04:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:06:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:08:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:09:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:11:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:13:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:15:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:17:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:18:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:19:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:21:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:23:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:25:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:27:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:29:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:31:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:32:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:33:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:35:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:37:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:39:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:40:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:42:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:44:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:46:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:47:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:49:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:51:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:52:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:54:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:56:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:58:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 06:59:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:01:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:03:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:04:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:06:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:08:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:10:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:12:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:13:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:15:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:17:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:18:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:19:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:21:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:22:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:24:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:25:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:27:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:29:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:30:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:31:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:33:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:34:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:36:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:38:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:39:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:41:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:42:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:44:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:45:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:47:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:48:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:50:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:51:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:53:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:54:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:56:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:58:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 07:59:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:00:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:02:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:03:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:05:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:06:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:08:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:09:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:10:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:11:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:13:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:14:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:15:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:17:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:18:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:19:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:21:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:22:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:23:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:24:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:26:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:27:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:28:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:30:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:31:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:33:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:34:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:35:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:36:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:38:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:39:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:40:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:42:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:43:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:44:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:45:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:47:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:48:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:50:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:51:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:52:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:53:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:54:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:56:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:57:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 08:59:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:00:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:01:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:02:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:04:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:05:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:06:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:08:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:09:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:10:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:11:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:13:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:14:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:15:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:17:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:18:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:19:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:21:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:22:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:23:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:25:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:26:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:28:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:29:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:30:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:32:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:33:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:34:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:35:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:37:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:38:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:39:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 09:40:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 19:46:09 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -5103,7 +6942,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1213</v>
+        <v>1825</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -5170,7 +7009,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1214</v>
+        <v>1826</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -5237,7 +7076,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1215</v>
+        <v>1827</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -5304,7 +7143,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1216</v>
+        <v>1828</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -5371,7 +7210,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1217</v>
+        <v>1829</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -5438,7 +7277,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1218</v>
+        <v>1830</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -5505,7 +7344,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1219</v>
+        <v>1831</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -5569,10 +7408,10 @@
     </row>
     <row ht="30" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1220</v>
+        <v>1832</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -5639,7 +7478,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1221</v>
+        <v>1833</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -5703,10 +7542,10 @@
     </row>
     <row ht="30" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>1222</v>
+        <v>1834</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -5773,7 +7612,7 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1223</v>
+        <v>1835</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -5840,7 +7679,7 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1224</v>
+        <v>1836</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -5907,7 +7746,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1225</v>
+        <v>1837</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -5974,7 +7813,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1226</v>
+        <v>1838</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -6041,7 +7880,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1227</v>
+        <v>1839</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -6108,7 +7947,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>1228</v>
+        <v>1840</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -6172,10 +8011,10 @@
     </row>
     <row ht="30" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1229</v>
+        <v>1841</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -6242,7 +8081,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1230</v>
+        <v>1842</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -6309,7 +8148,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1231</v>
+        <v>1843</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -6376,7 +8215,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1232</v>
+        <v>1844</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -6440,10 +8279,10 @@
     </row>
     <row ht="30" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>1233</v>
+        <v>1845</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -6510,7 +8349,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1234</v>
+        <v>1846</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -6577,7 +8416,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1235</v>
+        <v>1847</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -6644,7 +8483,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>1236</v>
+        <v>1848</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -6711,7 +8550,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1237</v>
+        <v>1849</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -6778,7 +8617,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1238</v>
+        <v>1850</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -6842,10 +8681,10 @@
     </row>
     <row ht="30" r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1239</v>
+        <v>1851</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -6912,7 +8751,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1240</v>
+        <v>1852</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -6976,10 +8815,10 @@
     </row>
     <row ht="30" r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1241</v>
+        <v>1853</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -7046,7 +8885,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1242</v>
+        <v>1854</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -7113,7 +8952,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1243</v>
+        <v>1855</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -7180,7 +9019,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1244</v>
+        <v>1856</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -7247,7 +9086,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1245</v>
+        <v>1857</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -7314,7 +9153,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>1246</v>
+        <v>1858</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -7381,7 +9220,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1247</v>
+        <v>1859</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -7445,10 +9284,10 @@
     </row>
     <row ht="30" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1248</v>
+        <v>1860</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -7515,7 +9354,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1249</v>
+        <v>1861</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -7579,10 +9418,10 @@
     </row>
     <row ht="30" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>1250</v>
+        <v>1862</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -7646,10 +9485,10 @@
     </row>
     <row ht="30" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1251</v>
+        <v>1863</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -7716,7 +9555,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1252</v>
+        <v>1864</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -7780,10 +9619,10 @@
     </row>
     <row ht="30" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1253</v>
+        <v>1865</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -7850,7 +9689,7 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>1254</v>
+        <v>1866</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -7917,7 +9756,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1255</v>
+        <v>1867</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -7984,7 +9823,7 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>1256</v>
+        <v>1868</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -8048,10 +9887,10 @@
     </row>
     <row ht="30" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>1257</v>
+        <v>1869</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -8115,10 +9954,10 @@
     </row>
     <row ht="30" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>1258</v>
+        <v>1870</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -8185,7 +10024,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1259</v>
+        <v>1871</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -8252,7 +10091,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1260</v>
+        <v>1872</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -8319,7 +10158,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>1261</v>
+        <v>1873</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>109</v>
@@ -8386,7 +10225,7 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>1262</v>
+        <v>1874</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>104</v>
@@ -8450,10 +10289,10 @@
     </row>
     <row ht="45" r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>1263</v>
+        <v>1875</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>110</v>
@@ -8647,7 +10486,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1456</v>
+        <v>2068</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -8712,10 +10551,10 @@
     </row>
     <row ht="60" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1457</v>
+        <v>2069</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -8783,7 +10622,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1458</v>
+        <v>2070</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -8848,10 +10687,10 @@
     </row>
     <row ht="60" r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1459</v>
+        <v>2071</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -8919,7 +10758,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1460</v>
+        <v>2072</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -8987,7 +10826,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1461</v>
+        <v>2073</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -9052,10 +10891,10 @@
     </row>
     <row ht="60" r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1462</v>
+        <v>2074</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -9123,7 +10962,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1463</v>
+        <v>2075</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -9188,10 +11027,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1464</v>
+        <v>2076</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -9509,7 +11348,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1465</v>
+        <v>2077</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -9577,7 +11416,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1466</v>
+        <v>2078</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -9642,10 +11481,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1467</v>
+        <v>2079</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -9713,7 +11552,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1468</v>
+        <v>2080</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -9781,7 +11620,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1469</v>
+        <v>2081</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -9849,7 +11688,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1470</v>
+        <v>2082</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -9917,7 +11756,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1471</v>
+        <v>2083</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -9982,10 +11821,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1472</v>
+        <v>2084</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -10053,7 +11892,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1473</v>
+        <v>2085</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -10371,7 +12210,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1474</v>
+        <v>2086</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -10439,7 +12278,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1475</v>
+        <v>2087</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -10507,7 +12346,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1476</v>
+        <v>2088</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -10575,7 +12414,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1477</v>
+        <v>2089</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -10643,7 +12482,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1478</v>
+        <v>2090</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -10711,7 +12550,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1479</v>
+        <v>2091</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -10779,7 +12618,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1480</v>
+        <v>2092</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -10847,7 +12686,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1481</v>
+        <v>2093</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -10915,7 +12754,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1482</v>
+        <v>2094</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -11235,10 +13074,10 @@
     </row>
     <row ht="60" r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1483</v>
+        <v>2095</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -11306,7 +13145,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1484</v>
+        <v>2096</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -11371,10 +13210,10 @@
     </row>
     <row ht="60" r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1485</v>
+        <v>2097</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -11442,7 +13281,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1486</v>
+        <v>2098</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -11510,7 +13349,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1487</v>
+        <v>2099</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -11578,7 +13417,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1488</v>
+        <v>2100</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -11643,10 +13482,10 @@
     </row>
     <row ht="60" r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1489</v>
+        <v>2101</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -11714,7 +13553,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1490</v>
+        <v>2102</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -11782,7 +13621,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1491</v>
+        <v>2103</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -12104,7 +13943,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1492</v>
+        <v>2104</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -12172,7 +14011,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1493</v>
+        <v>2105</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -12240,7 +14079,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1494</v>
+        <v>2106</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -12308,7 +14147,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1495</v>
+        <v>2107</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -12376,7 +14215,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1496</v>
+        <v>2108</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -12444,7 +14283,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1497</v>
+        <v>2109</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -12512,7 +14351,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1498</v>
+        <v>2110</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -12580,7 +14419,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1499</v>
+        <v>2111</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -12648,7 +14487,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1500</v>
+        <v>2112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -12963,10 +14802,10 @@
     </row>
     <row ht="60" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1501</v>
+        <v>2113</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -13034,7 +14873,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1502</v>
+        <v>2114</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -13099,10 +14938,10 @@
     </row>
     <row ht="60" r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1503</v>
+        <v>2115</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -13170,7 +15009,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1504</v>
+        <v>2116</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -13238,7 +15077,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1505</v>
+        <v>2117</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -13306,7 +15145,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1506</v>
+        <v>2118</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -13374,7 +15213,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1507</v>
+        <v>2119</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -13442,7 +15281,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1508</v>
+        <v>2120</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -13507,10 +15346,10 @@
     </row>
     <row ht="60" r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1509</v>
+        <v>2121</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -13828,7 +15667,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1510</v>
+        <v>2122</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -13896,7 +15735,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1511</v>
+        <v>2123</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -13964,7 +15803,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1512</v>
+        <v>2124</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -14032,7 +15871,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1513</v>
+        <v>2125</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -14100,7 +15939,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1514</v>
+        <v>2126</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -14168,7 +16007,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1515</v>
+        <v>2127</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -14236,7 +16075,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1516</v>
+        <v>2128</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -14304,7 +16143,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1517</v>
+        <v>2129</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -14372,7 +16211,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1518</v>
+        <v>2130</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>
@@ -14687,7 +16526,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1264</v>
+        <v>1876</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -14751,10 +16590,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1265</v>
+        <v>1877</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -14818,10 +16657,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1266</v>
+        <v>1878</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -14885,10 +16724,10 @@
     </row>
     <row ht="75" r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1267</v>
+        <v>1879</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -14955,7 +16794,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1268</v>
+        <v>1880</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -15022,7 +16861,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1269</v>
+        <v>1881</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -15089,7 +16928,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1270</v>
+        <v>1882</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -15156,7 +16995,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1271</v>
+        <v>1883</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -15223,7 +17062,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1272</v>
+        <v>1884</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -15287,10 +17126,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>1273</v>
+        <v>1885</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -15357,7 +17196,7 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1274</v>
+        <v>1886</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -15421,10 +17260,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1275</v>
+        <v>1887</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -15491,7 +17330,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1276</v>
+        <v>1888</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -15558,7 +17397,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1277</v>
+        <v>1889</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -15625,7 +17464,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1278</v>
+        <v>1890</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -15692,7 +17531,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>1279</v>
+        <v>1891</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -15759,7 +17598,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1280</v>
+        <v>1892</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -15826,7 +17665,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1281</v>
+        <v>1893</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -15890,10 +17729,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1282</v>
+        <v>1894</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -15960,7 +17799,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1283</v>
+        <v>1895</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -16027,7 +17866,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>1284</v>
+        <v>1896</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -16094,7 +17933,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1285</v>
+        <v>1897</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -16158,10 +17997,10 @@
     </row>
     <row ht="75" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1286</v>
+        <v>1898</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -16225,10 +18064,10 @@
     </row>
     <row ht="75" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>1287</v>
+        <v>1899</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -16295,7 +18134,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1288</v>
+        <v>1900</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -16362,7 +18201,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1289</v>
+        <v>1901</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -16429,7 +18268,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1290</v>
+        <v>1902</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -16496,7 +18335,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1291</v>
+        <v>1903</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -16563,7 +18402,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1292</v>
+        <v>1904</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -16630,7 +18469,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1293</v>
+        <v>1905</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -16697,7 +18536,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1294</v>
+        <v>1906</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -16764,7 +18603,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1295</v>
+        <v>1907</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -16831,7 +18670,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1296</v>
+        <v>1908</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -16898,7 +18737,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>1297</v>
+        <v>1909</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -16965,7 +18804,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1298</v>
+        <v>1910</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -17032,7 +18871,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1299</v>
+        <v>1911</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -17099,7 +18938,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1300</v>
+        <v>1912</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -17166,7 +19005,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>1301</v>
+        <v>1913</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -17230,10 +19069,10 @@
     </row>
     <row ht="75" r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1302</v>
+        <v>1914</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -17300,7 +19139,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1303</v>
+        <v>1915</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -17364,10 +19203,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1304</v>
+        <v>1916</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -17434,7 +19273,7 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>1305</v>
+        <v>1917</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -17501,7 +19340,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1306</v>
+        <v>1918</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -17565,10 +19404,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>1307</v>
+        <v>1919</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -17635,7 +19474,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>1308</v>
+        <v>1920</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -17699,10 +19538,10 @@
     </row>
     <row ht="75" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>1309</v>
+        <v>1921</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -17769,7 +19608,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1310</v>
+        <v>1922</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -17836,7 +19675,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1311</v>
+        <v>1923</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -17903,7 +19742,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>1312</v>
+        <v>1924</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -18097,7 +19936,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1313</v>
+        <v>1925</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -18164,7 +20003,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1314</v>
+        <v>1926</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -18231,7 +20070,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1315</v>
+        <v>1927</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -18298,7 +20137,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1316</v>
+        <v>1928</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -18365,7 +20204,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1317</v>
+        <v>1929</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -18432,7 +20271,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1318</v>
+        <v>1930</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -18496,10 +20335,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1319</v>
+        <v>1931</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -18566,7 +20405,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1320</v>
+        <v>1932</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -18630,10 +20469,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1321</v>
+        <v>1933</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -18700,7 +20539,7 @@
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>1322</v>
+        <v>1934</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -18764,10 +20603,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1323</v>
+        <v>1935</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -18831,10 +20670,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1324</v>
+        <v>1936</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -18901,7 +20740,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1325</v>
+        <v>1937</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -18968,7 +20807,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1326</v>
+        <v>1938</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -19035,7 +20874,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1327</v>
+        <v>1939</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -19102,7 +20941,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>1328</v>
+        <v>1940</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -19169,7 +21008,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1329</v>
+        <v>1941</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -19236,7 +21075,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1330</v>
+        <v>1942</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -19300,10 +21139,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1331</v>
+        <v>1943</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -19367,10 +21206,10 @@
     </row>
     <row ht="75" r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1332</v>
+        <v>1944</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -19434,10 +21273,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>1333</v>
+        <v>1945</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -19501,10 +21340,10 @@
     </row>
     <row ht="75" r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1334</v>
+        <v>1946</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -19571,7 +21410,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1335</v>
+        <v>1947</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -19635,10 +21474,10 @@
     </row>
     <row ht="75" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>1336</v>
+        <v>2131</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -19705,7 +21544,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1337</v>
+        <v>1949</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -19772,7 +21611,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1338</v>
+        <v>1950</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -19839,7 +21678,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1339</v>
+        <v>1951</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -19903,10 +21742,10 @@
     </row>
     <row ht="75" r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1340</v>
+        <v>1952</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -19973,7 +21812,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1341</v>
+        <v>1953</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -20037,10 +21876,10 @@
     </row>
     <row ht="75" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1342</v>
+        <v>1954</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -20107,7 +21946,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1343</v>
+        <v>1955</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -20174,7 +22013,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1344</v>
+        <v>1956</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -20241,7 +22080,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1345</v>
+        <v>1957</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -20308,7 +22147,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>1346</v>
+        <v>1958</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -20375,7 +22214,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1347</v>
+        <v>1959</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -20439,10 +22278,10 @@
     </row>
     <row ht="75" r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1348</v>
+        <v>1960</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -20509,7 +22348,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1349</v>
+        <v>1961</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -20576,7 +22415,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>1350</v>
+        <v>1962</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -20643,7 +22482,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1351</v>
+        <v>1963</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -20710,7 +22549,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1352</v>
+        <v>1964</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -20777,7 +22616,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1353</v>
+        <v>1965</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -20844,7 +22683,7 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>1354</v>
+        <v>1966</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -20911,7 +22750,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1355</v>
+        <v>1967</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -20975,10 +22814,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>1356</v>
+        <v>1968</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -21045,7 +22884,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>1357</v>
+        <v>1969</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -21109,10 +22948,10 @@
     </row>
     <row ht="75" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>1358</v>
+        <v>1970</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -21179,7 +23018,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1359</v>
+        <v>1971</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -21246,7 +23085,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1360</v>
+        <v>1972</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -21313,7 +23152,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>1361</v>
+        <v>1973</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -21506,7 +23345,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1362</v>
+        <v>1974</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -21573,7 +23412,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1363</v>
+        <v>1975</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -21640,7 +23479,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1364</v>
+        <v>1976</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -21707,7 +23546,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1365</v>
+        <v>1977</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -21774,7 +23613,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1366</v>
+        <v>1978</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -21841,7 +23680,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1367</v>
+        <v>1979</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -21908,7 +23747,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1368</v>
+        <v>1980</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -21975,7 +23814,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1369</v>
+        <v>1981</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -22042,7 +23881,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1370</v>
+        <v>1982</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -22109,7 +23948,7 @@
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>1371</v>
+        <v>1983</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -22176,7 +24015,7 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1372</v>
+        <v>1984</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -22243,7 +24082,7 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1373</v>
+        <v>1985</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -22310,7 +24149,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1374</v>
+        <v>1986</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -22377,7 +24216,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1375</v>
+        <v>1987</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -22444,7 +24283,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1376</v>
+        <v>1988</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -22511,7 +24350,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>1377</v>
+        <v>1989</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -22578,7 +24417,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1378</v>
+        <v>1990</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -22645,7 +24484,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1379</v>
+        <v>1991</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -22712,7 +24551,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1380</v>
+        <v>1992</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -22779,7 +24618,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1381</v>
+        <v>1993</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -22846,7 +24685,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>1382</v>
+        <v>1994</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -22913,7 +24752,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1383</v>
+        <v>1995</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -22980,7 +24819,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1384</v>
+        <v>1996</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -23047,7 +24886,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>1385</v>
+        <v>1997</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -23114,7 +24953,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1386</v>
+        <v>1998</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -23181,7 +25020,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1387</v>
+        <v>1999</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -23248,7 +25087,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1388</v>
+        <v>2000</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -23315,7 +25154,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1389</v>
+        <v>2001</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -23382,7 +25221,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1390</v>
+        <v>2002</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -23449,7 +25288,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1391</v>
+        <v>2003</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -23516,7 +25355,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1392</v>
+        <v>2004</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -23583,7 +25422,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1393</v>
+        <v>2005</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -23650,7 +25489,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1394</v>
+        <v>2006</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -23717,7 +25556,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>1395</v>
+        <v>2007</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -23784,7 +25623,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1396</v>
+        <v>2008</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -23851,7 +25690,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1397</v>
+        <v>2009</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -23918,7 +25757,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1398</v>
+        <v>2010</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -23985,7 +25824,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>1399</v>
+        <v>2011</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -24052,7 +25891,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1400</v>
+        <v>2012</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -24119,7 +25958,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1401</v>
+        <v>2013</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -24186,7 +26025,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1402</v>
+        <v>2014</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -24253,7 +26092,7 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>1403</v>
+        <v>2015</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -24320,7 +26159,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1404</v>
+        <v>2016</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -24387,7 +26226,7 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>1405</v>
+        <v>2017</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -24454,7 +26293,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>1406</v>
+        <v>2018</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -24521,7 +26360,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>1407</v>
+        <v>2019</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -24588,7 +26427,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1408</v>
+        <v>2020</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -24655,7 +26494,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1409</v>
+        <v>2021</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -24722,7 +26561,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>1410</v>
+        <v>2022</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -24916,10 +26755,10 @@
     </row>
     <row ht="75" r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1411</v>
+        <v>2023</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -24983,10 +26822,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1412</v>
+        <v>2024</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -25053,7 +26892,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1413</v>
+        <v>2025</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -25120,7 +26959,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1414</v>
+        <v>2026</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -25184,10 +27023,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1415</v>
+        <v>2027</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -25254,7 +27093,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1416</v>
+        <v>2028</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -25321,7 +27160,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1417</v>
+        <v>2029</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -25388,7 +27227,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1418</v>
+        <v>2030</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -25455,7 +27294,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1419</v>
+        <v>2031</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -25771,7 +27610,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1420</v>
+        <v>2032</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -25838,7 +27677,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1421</v>
+        <v>2033</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -25902,10 +27741,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1422</v>
+        <v>2034</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -25972,7 +27811,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1423</v>
+        <v>2035</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -26039,7 +27878,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1424</v>
+        <v>2036</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -26106,7 +27945,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1425</v>
+        <v>2037</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -26170,10 +28009,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1426</v>
+        <v>2038</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -26237,10 +28076,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1427</v>
+        <v>2039</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -26304,10 +28143,10 @@
     </row>
     <row ht="75" r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1428</v>
+        <v>2040</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -26624,7 +28463,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1429</v>
+        <v>2041</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -26688,10 +28527,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1430</v>
+        <v>2042</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -26755,10 +28594,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1431</v>
+        <v>2043</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -26825,7 +28664,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1432</v>
+        <v>2044</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -26889,10 +28728,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1433</v>
+        <v>2045</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -26959,7 +28798,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1434</v>
+        <v>2046</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -27026,7 +28865,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1435</v>
+        <v>2047</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -27090,10 +28929,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1436</v>
+        <v>2048</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -27160,7 +28999,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1437</v>
+        <v>2049</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -27477,7 +29316,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1438</v>
+        <v>2050</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -27544,7 +29383,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1439</v>
+        <v>2051</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -27611,7 +29450,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1440</v>
+        <v>2052</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -27678,7 +29517,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1441</v>
+        <v>2053</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -27745,7 +29584,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1442</v>
+        <v>2054</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -27812,7 +29651,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1443</v>
+        <v>2055</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -27879,7 +29718,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1444</v>
+        <v>2056</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
@@ -27946,7 +29785,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1445</v>
+        <v>2057</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -28013,7 +29852,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1446</v>
+        <v>2058</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
@@ -28331,7 +30170,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1447</v>
+        <v>2059</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>42</v>
@@ -28399,7 +30238,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1448</v>
+        <v>2060</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -28467,7 +30306,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1449</v>
+        <v>2061</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -28535,7 +30374,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1450</v>
+        <v>2062</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -28600,10 +30439,10 @@
     </row>
     <row ht="60" r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1451</v>
+        <v>2063</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
@@ -28668,10 +30507,10 @@
     </row>
     <row ht="60" r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1452</v>
+        <v>2064</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
@@ -28739,7 +30578,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1453</v>
+        <v>2065</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -28804,10 +30643,10 @@
     </row>
     <row ht="60" r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1454</v>
+        <v>2066</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -28875,7 +30714,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1455</v>
+        <v>2067</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Object Repo and Keywords done for BWP Bootstrap
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/DisplayCFData.xlsx
+++ b/KatalonData/IWPTestData/DisplayCFData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12032" uniqueCount="2132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12660" uniqueCount="2289">
   <si>
     <t>Result</t>
   </si>
@@ -6436,6 +6436,477 @@
   </si>
   <si>
     <t>Mon Sep 08 19:46:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:46:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:48:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:50:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:51:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:52:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:53:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:55:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:56:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:58:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 22:59:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:01:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:02:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:03:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:04:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:06:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:08:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:09:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:10:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:11:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:13:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:14:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:15:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:16:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:17:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:19:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:20:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:21:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:23:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:24:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:25:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:27:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:28:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:29:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:30:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:32:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:33:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:34:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:36:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:37:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:38:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:40:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:41:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:43:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:44:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:45:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:47:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:48:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:50:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:51:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:53:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:54:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:56:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:57:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Sep 08 23:58:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:00:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:01:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:02:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:04:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:06:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:07:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:08:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:10:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:11:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:13:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:14:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:16:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:17:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:19:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:20:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:22:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:23:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:25:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:26:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:27:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:29:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:30:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:31:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:32:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:34:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:35:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:36:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:38:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:39:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:41:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:42:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:44:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:45:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:46:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:48:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:50:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:51:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:53:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:54:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:56:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:57:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 00:58:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:00:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:01:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:02:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:04:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:06:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:07:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:08:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:10:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:11:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:13:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:14:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:15:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:16:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:18:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:19:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:21:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:23:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:24:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:25:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:27:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:29:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:31:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:32:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:34:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:35:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:37:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:38:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:40:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:41:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:43:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:44:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:45:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:47:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:48:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:49:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:50:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:51:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:53:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:54:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:55:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:56:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:57:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 01:59:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:00:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:02:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:03:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:04:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:07:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:09:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:11:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:12:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:14:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:15:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:16:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:17:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:19:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:21:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:22:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:24:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:26:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 09 02:27:48 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -6942,7 +7413,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1825</v>
+        <v>2132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -7009,7 +7480,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1826</v>
+        <v>2133</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -7076,7 +7547,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1827</v>
+        <v>2134</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -7143,7 +7614,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1828</v>
+        <v>2135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -7210,7 +7681,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1829</v>
+        <v>2136</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -7274,10 +7745,10 @@
     </row>
     <row ht="30" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>1830</v>
+        <v>2137</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -7344,7 +7815,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1831</v>
+        <v>2138</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -7411,7 +7882,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1832</v>
+        <v>2139</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -7478,7 +7949,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1833</v>
+        <v>2140</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -7542,10 +8013,10 @@
     </row>
     <row ht="30" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>1834</v>
+        <v>2141</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -7612,7 +8083,7 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1835</v>
+        <v>2142</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -7679,7 +8150,7 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1836</v>
+        <v>2143</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -7746,7 +8217,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1837</v>
+        <v>2144</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -7810,10 +8281,10 @@
     </row>
     <row ht="30" r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>1838</v>
+        <v>2145</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -7880,7 +8351,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1839</v>
+        <v>2146</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -7947,7 +8418,7 @@
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>1840</v>
+        <v>2147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -8014,7 +8485,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1841</v>
+        <v>2148</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -8081,7 +8552,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1842</v>
+        <v>2149</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -8148,7 +8619,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1843</v>
+        <v>2150</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -8215,7 +8686,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1844</v>
+        <v>2151</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -8282,7 +8753,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>1845</v>
+        <v>2152</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -8349,7 +8820,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1846</v>
+        <v>2153</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -8416,7 +8887,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1847</v>
+        <v>2154</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -8480,10 +8951,10 @@
     </row>
     <row ht="30" r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>1848</v>
+        <v>2155</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -8550,7 +9021,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1849</v>
+        <v>2156</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -8617,7 +9088,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1850</v>
+        <v>2157</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -8684,7 +9155,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1851</v>
+        <v>2158</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -8751,7 +9222,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1852</v>
+        <v>2159</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -8818,7 +9289,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1853</v>
+        <v>2160</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -8885,7 +9356,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1854</v>
+        <v>2161</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -8952,7 +9423,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1855</v>
+        <v>2162</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -9019,7 +9490,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1856</v>
+        <v>2163</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -9086,7 +9557,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1857</v>
+        <v>2164</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -9150,10 +9621,10 @@
     </row>
     <row ht="30" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>1858</v>
+        <v>2165</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -9220,7 +9691,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1859</v>
+        <v>2166</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -9287,7 +9758,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1860</v>
+        <v>2167</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -9354,7 +9825,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1861</v>
+        <v>2168</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -9421,7 +9892,7 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>1862</v>
+        <v>2169</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -9488,7 +9959,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1863</v>
+        <v>2170</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -9555,7 +10026,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1864</v>
+        <v>2171</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -9622,7 +10093,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1865</v>
+        <v>2172</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -9686,10 +10157,10 @@
     </row>
     <row ht="30" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>1866</v>
+        <v>2173</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -9756,7 +10227,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1867</v>
+        <v>2174</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -9820,10 +10291,10 @@
     </row>
     <row ht="30" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>1868</v>
+        <v>2175</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -9887,10 +10358,10 @@
     </row>
     <row ht="30" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>1869</v>
+        <v>2176</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -9954,10 +10425,10 @@
     </row>
     <row ht="30" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>1870</v>
+        <v>2177</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -10024,7 +10495,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1871</v>
+        <v>2178</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -10091,7 +10562,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1872</v>
+        <v>2179</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -10158,7 +10629,7 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>1873</v>
+        <v>2180</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>109</v>
@@ -10225,7 +10696,7 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>1874</v>
+        <v>2181</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>104</v>
@@ -10289,10 +10760,10 @@
     </row>
     <row ht="45" r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>1875</v>
+        <v>2182</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>110</v>
@@ -16526,7 +16997,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1876</v>
+        <v>2183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -16590,10 +17061,10 @@
     </row>
     <row ht="75" r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>1877</v>
+        <v>2184</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -16660,7 +17131,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1878</v>
+        <v>2185</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -16727,7 +17198,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1879</v>
+        <v>2186</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -16794,7 +17265,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1880</v>
+        <v>2187</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -16858,10 +17329,10 @@
     </row>
     <row ht="75" r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>1881</v>
+        <v>2188</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -16925,10 +17396,10 @@
     </row>
     <row ht="75" r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>1882</v>
+        <v>2189</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -16995,7 +17466,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1883</v>
+        <v>2190</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -17062,7 +17533,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1884</v>
+        <v>2191</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -17126,10 +17597,10 @@
     </row>
     <row ht="75" r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>1885</v>
+        <v>2192</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -17196,7 +17667,7 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>1886</v>
+        <v>2193</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -17260,10 +17731,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>1887</v>
+        <v>2194</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -17327,10 +17798,10 @@
     </row>
     <row ht="75" r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>1888</v>
+        <v>2195</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -17397,7 +17868,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1889</v>
+        <v>2196</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -17464,7 +17935,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>1890</v>
+        <v>2197</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -17528,10 +17999,10 @@
     </row>
     <row ht="75" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>1891</v>
+        <v>2198</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -17598,7 +18069,7 @@
         <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>1892</v>
+        <v>2199</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -17662,10 +18133,10 @@
     </row>
     <row ht="75" r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>1893</v>
+        <v>2200</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -17729,10 +18200,10 @@
     </row>
     <row ht="75" r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>1894</v>
+        <v>2201</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -17799,7 +18270,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1895</v>
+        <v>2202</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -17863,10 +18334,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>1896</v>
+        <v>2203</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -17933,7 +18404,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1897</v>
+        <v>2204</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -18000,7 +18471,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>1898</v>
+        <v>2205</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -18067,7 +18538,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>1899</v>
+        <v>2206</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -18134,7 +18605,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1900</v>
+        <v>2207</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -18201,7 +18672,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>1901</v>
+        <v>2208</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -18265,10 +18736,10 @@
     </row>
     <row ht="75" r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>1902</v>
+        <v>2209</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -18335,7 +18806,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1903</v>
+        <v>2210</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -18402,7 +18873,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1904</v>
+        <v>2211</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -18466,10 +18937,10 @@
     </row>
     <row ht="75" r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>1905</v>
+        <v>2212</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -18536,7 +19007,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1906</v>
+        <v>2213</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -18600,10 +19071,10 @@
     </row>
     <row ht="75" r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>1907</v>
+        <v>2214</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -18670,7 +19141,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1908</v>
+        <v>2215</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -18734,10 +19205,10 @@
     </row>
     <row ht="75" r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>1909</v>
+        <v>2216</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -18804,7 +19275,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>1910</v>
+        <v>2217</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -18871,7 +19342,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1911</v>
+        <v>2218</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -18935,10 +19406,10 @@
     </row>
     <row ht="75" r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>1912</v>
+        <v>2219</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -19002,10 +19473,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>1913</v>
+        <v>2220</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -19072,7 +19543,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1914</v>
+        <v>2221</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -19139,7 +19610,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>1915</v>
+        <v>2222</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -19203,10 +19674,10 @@
     </row>
     <row ht="75" r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>1916</v>
+        <v>2223</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -19270,10 +19741,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>1917</v>
+        <v>2224</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -19340,7 +19811,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>1918</v>
+        <v>2225</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -19407,7 +19878,7 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>1919</v>
+        <v>2226</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -19474,7 +19945,7 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>1920</v>
+        <v>2227</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -19538,10 +20009,10 @@
     </row>
     <row ht="75" r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>1921</v>
+        <v>2228</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -19608,7 +20079,7 @@
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>1922</v>
+        <v>2229</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -19672,10 +20143,10 @@
     </row>
     <row ht="75" r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>1923</v>
+        <v>2230</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -19739,10 +20210,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>1924</v>
+        <v>2231</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -19936,7 +20407,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1925</v>
+        <v>2232</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -20003,7 +20474,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1926</v>
+        <v>2233</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -20067,10 +20538,10 @@
     </row>
     <row ht="75" r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>1927</v>
+        <v>2234</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -20137,7 +20608,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1928</v>
+        <v>2235</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -20201,10 +20672,10 @@
     </row>
     <row ht="75" r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>1929</v>
+        <v>2236</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -20271,7 +20742,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1930</v>
+        <v>2237</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -20338,7 +20809,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1931</v>
+        <v>2238</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -20402,10 +20873,10 @@
     </row>
     <row ht="75" r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>1932</v>
+        <v>2239</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -20472,7 +20943,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>1933</v>
+        <v>2240</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -20539,7 +21010,7 @@
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>1934</v>
+        <v>2241</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -20603,10 +21074,10 @@
     </row>
     <row ht="75" r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>1935</v>
+        <v>2242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
@@ -20670,10 +21141,10 @@
     </row>
     <row ht="75" r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>1936</v>
+        <v>2243</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -20740,7 +21211,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>1937</v>
+        <v>2244</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -20807,7 +21278,7 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>1938</v>
+        <v>2245</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -20871,10 +21342,10 @@
     </row>
     <row ht="75" r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>1939</v>
+        <v>2246</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -20938,10 +21409,10 @@
     </row>
     <row ht="75" r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>1940</v>
+        <v>2247</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -21005,10 +21476,10 @@
     </row>
     <row ht="75" r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>1941</v>
+        <v>2248</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -21075,7 +21546,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1942</v>
+        <v>2249</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -21142,7 +21613,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>1943</v>
+        <v>2250</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -21209,7 +21680,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>1944</v>
+        <v>2251</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
@@ -21273,10 +21744,10 @@
     </row>
     <row ht="75" r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>1945</v>
+        <v>2252</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -21343,7 +21814,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>1946</v>
+        <v>2253</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -21407,10 +21878,10 @@
     </row>
     <row ht="75" r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>1947</v>
+        <v>2254</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -21477,7 +21948,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>2131</v>
+        <v>2255</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
@@ -21544,7 +22015,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>1949</v>
+        <v>2256</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
@@ -21608,10 +22079,10 @@
     </row>
     <row ht="75" r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>1950</v>
+        <v>2257</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
@@ -21678,7 +22149,7 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>1951</v>
+        <v>2258</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -21745,7 +22216,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>1952</v>
+        <v>2259</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
@@ -21812,7 +22283,7 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>1953</v>
+        <v>2260</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
@@ -21879,7 +22350,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>1954</v>
+        <v>2261</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>28</v>
@@ -21946,7 +22417,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>1955</v>
+        <v>2262</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>28</v>
@@ -22013,7 +22484,7 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>1956</v>
+        <v>2263</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>28</v>
@@ -22080,7 +22551,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>1957</v>
+        <v>2264</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>28</v>
@@ -22147,7 +22618,7 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>1958</v>
+        <v>2265</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -22211,10 +22682,10 @@
     </row>
     <row ht="75" r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>1959</v>
+        <v>2266</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>28</v>
@@ -22281,7 +22752,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>1960</v>
+        <v>2267</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -22348,7 +22819,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1961</v>
+        <v>2268</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -22412,10 +22883,10 @@
     </row>
     <row ht="75" r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>1962</v>
+        <v>2269</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>28</v>
@@ -22482,7 +22953,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>1963</v>
+        <v>2270</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -22546,10 +23017,10 @@
     </row>
     <row ht="75" r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>1964</v>
+        <v>2271</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>28</v>
@@ -22616,7 +23087,7 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>1965</v>
+        <v>2272</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>28</v>
@@ -22680,10 +23151,10 @@
     </row>
     <row ht="75" r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>1966</v>
+        <v>2273</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>28</v>
@@ -22747,10 +23218,10 @@
     </row>
     <row ht="75" r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>1967</v>
+        <v>2274</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>28</v>
@@ -22814,10 +23285,10 @@
     </row>
     <row ht="75" r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>1968</v>
+        <v>2275</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>28</v>
@@ -22881,10 +23352,10 @@
     </row>
     <row ht="75" r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>1969</v>
+        <v>2276</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>28</v>
@@ -22951,7 +23422,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>1970</v>
+        <v>2277</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>28</v>
@@ -23015,10 +23486,10 @@
     </row>
     <row ht="75" r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>1971</v>
+        <v>2278</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -23085,7 +23556,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>1972</v>
+        <v>2279</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>28</v>
@@ -23149,10 +23620,10 @@
     </row>
     <row ht="75" r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>1973</v>
+        <v>2280</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -23345,7 +23816,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>1974</v>
+        <v>2281</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -23412,7 +23883,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>1975</v>
+        <v>2282</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -23479,7 +23950,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>1976</v>
+        <v>2283</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -23546,7 +24017,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>1977</v>
+        <v>2284</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -23613,7 +24084,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>1978</v>
+        <v>2285</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -23680,7 +24151,7 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>1979</v>
+        <v>2286</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -23747,7 +24218,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>1980</v>
+        <v>2287</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -23814,7 +24285,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1981</v>
+        <v>2288</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>

</xml_diff>